<commit_message>
revised display code to add in fram for transposition and reformatted the sensor adjustments
</commit_message>
<xml_diff>
--- a/Documentation/FRAM data storage addresses.xlsx
+++ b/Documentation/FRAM data storage addresses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\OneDrive\Documents\Arduino\MidiEvi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\OneDrive\Documents\Arduino\MidiEvi\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F12BE1-559B-46A2-B9BD-8300D611906F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E529F683-88FF-4720-B45F-C3EFCAA10978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{F8769F7E-5CC2-4571-805C-FB882DD6C7E6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>A</t>
   </si>
@@ -184,6 +184,15 @@
   </si>
   <si>
     <t>Rotator 4 Chord Values</t>
+  </si>
+  <si>
+    <t>Sensor THR and MAX storage (Pressure, Pbup, Pbdown, Bite, ExtraMod) (THR, MAX)</t>
+  </si>
+  <si>
+    <t>Sensor Range THR and MAX storage (Pressure, Pbup, Pbdown, Bite, ExtraMod) (THR, MAX) (Static)</t>
+  </si>
+  <si>
+    <t>Transposition Number</t>
   </si>
 </sst>
 </file>
@@ -219,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -232,6 +241,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -550,7 +562,7 @@
   <dimension ref="A1:P65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -655,49 +667,53 @@
       <c r="A4">
         <v>20</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
+      <c r="B4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>30</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
+      <c r="B5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>40</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -717,7 +733,9 @@
       <c r="A7">
         <v>50</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -1690,11 +1708,21 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="23">
+    <mergeCell ref="B2:P3"/>
+    <mergeCell ref="B18:P19"/>
+    <mergeCell ref="B20:P21"/>
+    <mergeCell ref="B22:P23"/>
+    <mergeCell ref="B24:P25"/>
+    <mergeCell ref="B14:P15"/>
+    <mergeCell ref="B16:P17"/>
+    <mergeCell ref="B4:P4"/>
+    <mergeCell ref="B5:P5"/>
+    <mergeCell ref="B7:P13"/>
+    <mergeCell ref="C6:P6"/>
     <mergeCell ref="B44:P45"/>
     <mergeCell ref="B46:P47"/>
     <mergeCell ref="B48:P49"/>
-    <mergeCell ref="B4:P13"/>
     <mergeCell ref="B34:P35"/>
     <mergeCell ref="B36:P37"/>
     <mergeCell ref="B38:P39"/>
@@ -1704,13 +1732,6 @@
     <mergeCell ref="B28:P29"/>
     <mergeCell ref="B30:P31"/>
     <mergeCell ref="B32:P33"/>
-    <mergeCell ref="B2:P3"/>
-    <mergeCell ref="B18:P19"/>
-    <mergeCell ref="B20:P21"/>
-    <mergeCell ref="B22:P23"/>
-    <mergeCell ref="B24:P25"/>
-    <mergeCell ref="B14:P15"/>
-    <mergeCell ref="B16:P17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Started on menu class and testing out teensy features
</commit_message>
<xml_diff>
--- a/Documentation/FRAM data storage addresses.xlsx
+++ b/Documentation/FRAM data storage addresses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\OneDrive\Documents\Arduino\MidiEvi\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4CC301-1A83-41ED-8B91-2E707527A866}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2621B1DE-4868-4416-8AAA-8E118CCDE71D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{F8769F7E-5CC2-4571-805C-FB882DD6C7E6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>A</t>
   </si>
@@ -132,12 +132,6 @@
     <t>UNUSED RESET CHORD VALUE</t>
   </si>
   <si>
-    <t>160 BYTES EMPTY FOR FUTURE VARIABLE STORAGE</t>
-  </si>
-  <si>
-    <t>Reserved for test and System Storage</t>
-  </si>
-  <si>
     <t>2A0</t>
   </si>
   <si>
@@ -193,6 +187,15 @@
   </si>
   <si>
     <t>Breath Curve (Type, Log, Exp, Sin)</t>
+  </si>
+  <si>
+    <t>80 BYTES EMPTY FOR FUTURE VARIABLE STORAGE</t>
+  </si>
+  <si>
+    <t>Reserved for testing and System Storage</t>
+  </si>
+  <si>
+    <t>MIDI Controls (Channel; Lead, Chord Velocity; CC resolution in bits; Pressure, PitchBend, Portamento, Extra Controller CC)</t>
   </si>
 </sst>
 </file>
@@ -228,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -245,6 +248,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -560,74 +569,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D039B4F-63A3-455E-9E01-3DE6FFE9292C}">
-  <dimension ref="A1:P65"/>
+  <dimension ref="A1:S65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:F8"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.59765625" customWidth="1"/>
-    <col min="2" max="2" width="9.06640625" customWidth="1"/>
+    <col min="1" max="2" width="10.59765625" customWidth="1"/>
+    <col min="3" max="3" width="9.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>18</v>
       </c>
       <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="D1">
         <v>2</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>3</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>4</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <v>5</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <v>6</v>
       </c>
-      <c r="H1">
+      <c r="I1">
         <v>7</v>
       </c>
-      <c r="I1">
+      <c r="J1">
         <v>8</v>
       </c>
-      <c r="J1">
+      <c r="K1">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -643,8 +655,9 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q2" s="5"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>10</v>
       </c>
@@ -663,13 +676,14 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q3" s="5"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>20</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -685,8 +699,9 @@
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q4" s="6"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>30</v>
       </c>
@@ -705,8 +720,9 @@
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q5" s="6"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>40</v>
       </c>
@@ -725,8 +741,9 @@
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q6" s="6"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>50</v>
       </c>
@@ -745,37 +762,40 @@
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q7" s="6"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>60</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
+      <c r="G8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
       <c r="P8" s="3"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q8" s="3"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>70</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -791,8 +811,9 @@
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q9" s="6"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>80</v>
       </c>
@@ -811,8 +832,9 @@
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q10" s="6"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>90</v>
       </c>
@@ -831,8 +853,9 @@
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q11" s="6"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -851,8 +874,10 @@
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q12" s="6"/>
+      <c r="S12" s="8"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -871,8 +896,9 @@
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q13" s="6"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -893,8 +919,9 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q14" s="5"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -913,8 +940,9 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q15" s="5"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -935,8 +963,9 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q16" s="5"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -955,8 +984,9 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q17" s="5"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>100</v>
       </c>
@@ -977,8 +1007,9 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q18" s="5"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>110</v>
       </c>
@@ -997,8 +1028,9 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q19" s="5"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>120</v>
       </c>
@@ -1019,8 +1051,9 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q20" s="5"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>130</v>
       </c>
@@ -1039,8 +1072,9 @@
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q21" s="5"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>140</v>
       </c>
@@ -1061,8 +1095,9 @@
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q22" s="5"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>150</v>
       </c>
@@ -1081,8 +1116,9 @@
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q23" s="5"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>160</v>
       </c>
@@ -1103,8 +1139,9 @@
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q24" s="5"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>170</v>
       </c>
@@ -1123,13 +1160,14 @@
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q25" s="5"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>180</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -1145,8 +1183,9 @@
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q26" s="5"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>190</v>
       </c>
@@ -1165,13 +1204,14 @@
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q27" s="5"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -1187,8 +1227,9 @@
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q28" s="5"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>13</v>
       </c>
@@ -1207,13 +1248,14 @@
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q29" s="5"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1229,8 +1271,9 @@
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q30" s="5"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>15</v>
       </c>
@@ -1249,13 +1292,14 @@
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q31" s="5"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1271,8 +1315,9 @@
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q32" s="5"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>16</v>
       </c>
@@ -1291,8 +1336,9 @@
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q33" s="5"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>200</v>
       </c>
@@ -1313,8 +1359,9 @@
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q34" s="5"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>210</v>
       </c>
@@ -1333,8 +1380,9 @@
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q35" s="5"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>220</v>
       </c>
@@ -1355,8 +1403,9 @@
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q36" s="5"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>230</v>
       </c>
@@ -1375,8 +1424,9 @@
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q37" s="5"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>240</v>
       </c>
@@ -1397,8 +1447,9 @@
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q38" s="5"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>250</v>
       </c>
@@ -1417,8 +1468,9 @@
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q39" s="5"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>260</v>
       </c>
@@ -1439,8 +1491,9 @@
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q40" s="5"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>270</v>
       </c>
@@ -1459,8 +1512,9 @@
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
       <c r="P41" s="5"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q41" s="5"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>280</v>
       </c>
@@ -1481,8 +1535,9 @@
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
       <c r="P42" s="5"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q42" s="5"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>290</v>
       </c>
@@ -1501,10 +1556,11 @@
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
       <c r="P43" s="5"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q43" s="5"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>28</v>
@@ -1523,10 +1579,11 @@
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
       <c r="P44" s="5"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q44" s="5"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -1543,10 +1600,11 @@
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
       <c r="P45" s="5"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q45" s="5"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>29</v>
@@ -1565,10 +1623,11 @@
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
       <c r="P46" s="5"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q46" s="5"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -1585,10 +1644,11 @@
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
       <c r="P47" s="5"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q47" s="5"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>30</v>
@@ -1607,10 +1667,11 @@
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
       <c r="P48" s="5"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q48" s="5"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -1627,111 +1688,119 @@
       <c r="N49" s="5"/>
       <c r="O49" s="5"/>
       <c r="P49" s="5"/>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q49" s="5"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>300</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>310</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>320</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>330</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>340</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>350</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>360</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>370</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>380</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>390</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A61" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A62" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A61" s="1" t="s">
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A63" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A62" s="1" t="s">
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A64" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A63" s="1" t="s">
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A65" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A64" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A65" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="B65" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="B26:P27"/>
-    <mergeCell ref="B28:P29"/>
-    <mergeCell ref="B30:P31"/>
-    <mergeCell ref="B32:P33"/>
-    <mergeCell ref="B4:P7"/>
-    <mergeCell ref="B9:P13"/>
+  <mergeCells count="23">
+    <mergeCell ref="B34:Q35"/>
+    <mergeCell ref="B36:Q37"/>
+    <mergeCell ref="B38:Q39"/>
+    <mergeCell ref="B40:Q41"/>
+    <mergeCell ref="B42:Q43"/>
+    <mergeCell ref="B18:Q19"/>
+    <mergeCell ref="B20:Q21"/>
+    <mergeCell ref="B22:Q23"/>
+    <mergeCell ref="B24:Q25"/>
+    <mergeCell ref="B26:Q27"/>
     <mergeCell ref="C8:F8"/>
-    <mergeCell ref="B44:P45"/>
-    <mergeCell ref="B46:P47"/>
-    <mergeCell ref="B48:P49"/>
-    <mergeCell ref="B34:P35"/>
-    <mergeCell ref="B36:P37"/>
-    <mergeCell ref="B38:P39"/>
-    <mergeCell ref="B40:P41"/>
-    <mergeCell ref="B42:P43"/>
-    <mergeCell ref="B2:P3"/>
-    <mergeCell ref="B18:P19"/>
-    <mergeCell ref="B20:P21"/>
-    <mergeCell ref="B22:P23"/>
-    <mergeCell ref="B24:P25"/>
-    <mergeCell ref="B14:P15"/>
-    <mergeCell ref="B16:P17"/>
+    <mergeCell ref="G8:N8"/>
+    <mergeCell ref="B2:Q3"/>
+    <mergeCell ref="B4:Q7"/>
+    <mergeCell ref="B9:Q13"/>
+    <mergeCell ref="B14:Q15"/>
+    <mergeCell ref="B16:Q17"/>
+    <mergeCell ref="B44:Q45"/>
+    <mergeCell ref="B46:Q47"/>
+    <mergeCell ref="B48:Q49"/>
+    <mergeCell ref="B28:Q29"/>
+    <mergeCell ref="B30:Q31"/>
+    <mergeCell ref="B32:Q33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>